<commit_message>
JST Updated in Main B
</commit_message>
<xml_diff>
--- a/Florian_PCB/LED_Ring/Production_Files/BOM-LESRv1.0.xlsx
+++ b/Florian_PCB/LED_Ring/Production_Files/BOM-LESRv1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eagle_projects_directory\Florian_PCB\LED_Ring\Production_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9242B7-15B8-4EB6-8CCE-74415D5D86D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4403AB3-90F8-4044-8D3C-7E79A9DC3919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Item #</t>
   </si>
@@ -277,14 +277,29 @@
     <t>Shape of the PCB - Circular (Diameter - 40mm)</t>
   </si>
   <si>
-    <t>R1,R2,R3,R4</t>
+    <t>R1,R2,R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>RC0402JR-07470RL</t>
+  </si>
+  <si>
+    <t>RES SMD 470 OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.in/short/z4hjwh </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +397,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -439,7 +460,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -524,6 +545,26 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -846,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I25"/>
+  <dimension ref="A2:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -867,27 +908,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="D2" s="33" t="s">
+      <c r="B2" s="44"/>
+      <c r="D2" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -1064,107 +1105,136 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.4">
-      <c r="A12" s="11">
+      <c r="A12" s="32">
         <v>6</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="31">
+        <v>1</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.4">
+      <c r="A13" s="11">
+        <v>7</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C13" s="7">
         <v>3</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G13" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I13" s="19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="B14" s="24" t="s">
+    <row r="15" spans="1:9">
+      <c r="B15" s="24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.4">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-    </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="14.4">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="1:9" ht="14.4">
-      <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="B18" s="24" t="s">
-        <v>46</v>
-      </c>
+    <row r="16" spans="1:9" ht="14.4">
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" ht="14.4">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" ht="14.4">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
     </row>
     <row r="19" spans="1:9">
       <c r="B19" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="B20" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="B21" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="B22" s="24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="2" customFormat="1" ht="14.4">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+    <row r="26" spans="1:9" s="2" customFormat="1" ht="14.4">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A18:I18"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
@@ -1172,8 +1242,9 @@
   <hyperlinks>
     <hyperlink ref="I7" r:id="rId1" xr:uid="{08754D15-7B9B-4752-A9E3-03D67A198B3B}"/>
     <hyperlink ref="I11" r:id="rId2" xr:uid="{D94B5E1C-82E2-449B-95C5-F73B47B8D66A}"/>
+    <hyperlink ref="I12" r:id="rId3" xr:uid="{36FA86D4-4066-455D-A648-8982420352F7}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>